<commit_message>
Updated PPMProposalSearch function to look for the text Saved Searches to know Search click worked and commented .sync after that to prevent PPM from auto closing the menu popup Corrected inaccurate comment Removed unused function Added function comments Updated OR to have more logical names
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-finance-review/Default.xlsx
+++ b/uft-one-ppm-build-finance-review/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Added steps to add projected financial costs into the Financial Summary
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-finance-review/Default.xlsx
+++ b/uft-one-ppm-build-finance-review/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Updated steps that weren't working on lower resolutions
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-finance-review/Default.xlsx
+++ b/uft-one-ppm-build-finance-review/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Updated for missing step of saving the changes to the financial details before closing and associate .sync
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-finance-review/Default.xlsx
+++ b/uft-one-ppm-build-finance-review/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Added a .highlight for the Save and Done objects on the edit costs window as PPM isn't saving fast enough
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-finance-review/Default.xlsx
+++ b/uft-one-ppm-build-finance-review/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Removed the .highlight steps added in previous update.  Edited object properties to include outerhtml which changes between enabled and disabled and added logic to wait for the enabled version to disappear before proceeding.
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-finance-review/Default.xlsx
+++ b/uft-one-ppm-build-finance-review/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Added logic to check to make sure the new cost value was successfully entered, if not, try again, up to 3 times.
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-finance-review/Default.xlsx
+++ b/uft-one-ppm-build-finance-review/Default.xlsx
@@ -212,10 +212,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -525,10 +525,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -543,10 +543,10 @@
       </c>
     </row>
     <row>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
-      <c s="1" t="s">
+      <c s="2" t="s">
         <v>3</v>
       </c>
       <c s="3"/>
@@ -566,7 +566,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Added parameter for the fiscal year to modify for costs
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-finance-review/Default.xlsx
+++ b/uft-one-ppm-build-finance-review/Default.xlsx
@@ -15,12 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>BrowserName</t>
   </si>
   <si>
     <t>CHROME</t>
+  </si>
+  <si>
+    <t>FiscalYear</t>
   </si>
   <si>
     <t>dtFirstReqID</t>
@@ -212,10 +215,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -517,18 +520,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.40234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.40234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.41796875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
@@ -536,20 +540,26 @@
         <v>0</v>
       </c>
       <c t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c t="s">
+        <v>3</v>
       </c>
       <c t="s">
         <v>2</v>
       </c>
     </row>
     <row>
-      <c s="2" t="s">
+      <c s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" t="s">
-        <v>3</v>
-      </c>
-      <c s="3"/>
+      <c s="1" t="s">
+        <v>4</v>
+      </c>
+      <c s="1"/>
+      <c s="3">
+        <v>2020</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -566,7 +576,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1"/>

</xml_diff>

<commit_message>
Modified the fiscal year parameter to be 2021, in 9.63 container the time machine has been run. This version will FAIL in 9.62.
</commit_message>
<xml_diff>
--- a/uft-one-ppm-build-finance-review/Default.xlsx
+++ b/uft-one-ppm-build-finance-review/Default.xlsx
@@ -523,7 +523,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -558,7 +558,7 @@
       </c>
       <c s="1"/>
       <c s="3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>